<commit_message>
Clustering MALI and Fe#
-rescaling + incorporating the time
-will look tomorrow if any trends could be unraveled, but wasn't the case on fist sight
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/Frost/Fe/control_points_count.xlsx
+++ b/_CLUSTER/groups_time_area/Frost/Fe/control_points_count.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -376,15 +376,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2633</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>1625</v>
+      <c r="B4" t="n">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cluster analysis control points: last cases
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/Frost/Fe/control_points_count.xlsx
+++ b/_CLUSTER/groups_time_area/Frost/Fe/control_points_count.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -376,31 +376,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1328</v>
+        <v>3051</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1272</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>766</v>
+        <v>1207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cluster analysis Birch+K_means method
same general information is obtained by the two methods: all areas are quite similar, except for area1 which is slightly different (following the trend of the other cluster analysis)
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/Frost/Fe/control_points_count.xlsx
+++ b/_CLUSTER/groups_time_area/Frost/Fe/control_points_count.xlsx
@@ -376,7 +376,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3051</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="3">
@@ -384,7 +384,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1207</v>
+        <v>1618</v>
       </c>
     </row>
   </sheetData>

</xml_diff>